<commit_message>
feat: added notes for Course 1 Module 2
</commit_message>
<xml_diff>
--- a/excel-basics/formula-functions/notes.xlsx
+++ b/excel-basics/formula-functions/notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\power-bi-cert\excel-basics\formula-functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0AF7FF-5668-4EA0-9021-6226A494BC8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8803A7A9-718E-423A-A151-24F0A82110BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="4" xr2:uid="{0D076788-1608-43AF-9E52-FBAA486EFBE6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="5" xr2:uid="{0D076788-1608-43AF-9E52-FBAA486EFBE6}"/>
   </bookViews>
   <sheets>
     <sheet name="chaining calculations" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="cell reference" sheetId="3" r:id="rId3"/>
     <sheet name="aboslute reference syntax" sheetId="5" r:id="rId4"/>
     <sheet name="conditional function formulas" sheetId="6" r:id="rId5"/>
+    <sheet name="SUMPRODUCT" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -735,8 +736,83 @@
 </comments>
 </file>
 
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Asus</author>
+  </authors>
+  <commentList>
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{AFE3CE9A-AE65-4891-99C2-8EA21347658E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">1. Type SUMPRODUCT
+2. Select A3:A4 </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(col1)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+3. Hold Ctrl, select B3:B4 </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(col2)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+4. Complete formula
+This calculates the sum of </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>col1 * col2</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>rel 1</t>
   </si>
@@ -788,12 +864,21 @@
   <si>
     <t>sum if no</t>
   </si>
+  <si>
+    <t>SUM of A * B</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -829,6 +914,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -838,7 +931,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -861,12 +954,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -877,6 +979,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1959,7 +2067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CBD423E-0594-493B-8568-7AF638D5F8A2}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -2086,4 +2194,64 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD42BF8-1E66-47A7-956B-E91B607C4D3F}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <f>SUMPRODUCT(A3:A4,B3:B4)</f>
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>